<commit_message>
Update of Application Profile with transliterations
</commit_message>
<xml_diff>
--- a/application-profile-update/ISSN-Modele-v2.xlsx
+++ b/application-profile-update/ISSN-Modele-v2.xlsx
@@ -310,10 +310,10 @@
     <t xml:space="preserve">022$a, 022$l, 030$a, 210$a, 222$a</t>
   </si>
   <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>rdfs:label</t>
+    <t xml:space="preserve">main title</t>
+  </si>
+  <si>
+    <t>bf:mainTitle</t>
   </si>
   <si>
     <t>xsd:string</t>
@@ -1385,6 +1385,12 @@
     <t>http://issn.org/resource/ISSN/{ISSN}#ReproductionPlace-{placeName}</t>
   </si>
   <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
     <t xml:space="preserve">This property contains the name of the place (generally a city).</t>
   </si>
   <si>
@@ -1581,12 +1587,6 @@
   </si>
   <si>
     <t xml:space="preserve">blank nodes for the Variant titles and Parallel titles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">main title</t>
-  </si>
-  <si>
-    <t>bf:mainTitle</t>
   </si>
   <si>
     <t>rdf:langString</t>
@@ -2206,7 +2206,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2223,12 +2223,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor theme="6" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="5"/>
-        <bgColor indexed="5"/>
       </patternFill>
     </fill>
     <fill>
@@ -2422,7 +2416,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="115">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2485,10 +2479,7 @@
     <xf fontId="0" fillId="0" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="4" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2500,8 +2491,7 @@
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="3" fillId="0" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2514,7 +2504,7 @@
     <xf fontId="1" fillId="0" borderId="9" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2580,7 +2570,7 @@
     <xf fontId="0" fillId="0" borderId="8" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2592,7 +2582,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -2604,7 +2594,7 @@
     </xf>
     <xf fontId="1" fillId="0" borderId="5" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf fontId="5" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="0" fillId="6" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2617,40 +2607,19 @@
     <xf fontId="3" fillId="0" borderId="8" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="2" fillId="4" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="4" borderId="9" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="4" borderId="8" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="4" borderId="8" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3431,7 +3400,7 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
       <selection activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -3443,63 +3412,63 @@
     <col customWidth="1" min="4" max="4" style="8" width="36.85546875"/>
     <col customWidth="1" min="5" max="5" width="11.5703125"/>
     <col customWidth="1" hidden="1" min="6" max="6" style="9" width="53"/>
-    <col customWidth="1" min="7" max="7" style="44" width="13.28515625"/>
+    <col customWidth="1" min="7" max="7" style="42" width="13.28515625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="75" t="s">
-        <v>485</v>
+      <c r="B3" s="73" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="75" t="s">
-        <v>486</v>
+      <c r="B4" s="73" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="75" t="s">
-        <v>487</v>
+      <c r="B5" s="73" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="75" t="s">
-        <v>488</v>
+      <c r="B6" s="73" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" s="4" customFormat="1">
@@ -3525,21 +3494,21 @@
         <v>58</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="10" s="18" customFormat="1" ht="57">
-      <c r="A10" s="65" t="s">
-        <v>491</v>
+      <c r="A10" s="63" t="s">
+        <v>493</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>492</v>
-      </c>
-      <c r="C10" s="81" t="s">
+        <v>494</v>
+      </c>
+      <c r="C10" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="82" t="s">
-        <v>493</v>
+      <c r="D10" s="80" t="s">
+        <v>495</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>94</v>
@@ -3548,49 +3517,49 @@
         <v>135</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" s="23" customFormat="1" ht="57">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="71" t="s">
         <v>415</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>416</v>
       </c>
-      <c r="C11" s="81" t="s">
-        <v>495</v>
+      <c r="C11" s="79" t="s">
+        <v>497</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="F11" s="83"/>
+        <v>499</v>
+      </c>
+      <c r="F11" s="81"/>
       <c r="G11" s="27" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="12" ht="57">
       <c r="A12" s="24" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="E12" s="25" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="25"/>
       <c r="G12" s="27" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="H12" t="s">
         <v>395</v>
@@ -3598,70 +3567,70 @@
     </row>
     <row r="13" ht="42.75">
       <c r="A13" s="24" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E13" s="25" t="s">
         <v>64</v>
       </c>
       <c r="F13" s="25"/>
       <c r="G13" s="27" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="H13" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="75" t="s">
-        <v>488</v>
+      <c r="B18" s="73" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="75" t="s">
-        <v>489</v>
+      <c r="B19" s="73" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="1">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="76" t="s">
-        <v>510</v>
+      <c r="B20" s="74" t="s">
+        <v>512</v>
       </c>
       <c r="D20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="44"/>
+      <c r="G20" s="42"/>
       <c r="H20" s="4" t="s">
         <v>373</v>
       </c>
@@ -3669,7 +3638,7 @@
     <row r="21" s="18" customFormat="1">
       <c r="D21" s="8"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="44"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="18" t="s">
         <v>380</v>
       </c>
@@ -3701,16 +3670,16 @@
       </c>
     </row>
     <row r="23" ht="128.25">
-      <c r="A23" s="84" t="s">
-        <v>511</v>
-      </c>
-      <c r="B23" s="85" t="s">
-        <v>512</v>
-      </c>
-      <c r="C23" s="85" t="s">
+      <c r="A23" s="63" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="D23" s="82" t="s">
+      <c r="D23" s="80" t="s">
         <v>514</v>
       </c>
       <c r="E23" s="20" t="s">
@@ -3722,7 +3691,7 @@
       </c>
     </row>
     <row r="24" ht="128.25">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="71" t="s">
         <v>515</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -3745,25 +3714,25 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="86" t="s">
+      <c r="A25" s="71" t="s">
         <v>347</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="D25" s="87" t="s">
+      <c r="D25" s="82" t="s">
         <v>521</v>
       </c>
-      <c r="E25" s="88" t="s">
+      <c r="E25" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="89" t="s">
+      <c r="F25" s="27" t="s">
         <v>518</v>
       </c>
-      <c r="G25" s="89"/>
+      <c r="G25" s="27"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3801,7 +3770,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -3809,7 +3778,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -3817,34 +3786,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="6" s="5" customFormat="1">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="73" t="s">
         <v>526</v>
       </c>
       <c r="C6" s="8"/>
@@ -3884,24 +3853,24 @@
         <v>373</v>
       </c>
     </row>
-    <row r="10" s="18" customFormat="1" ht="57">
-      <c r="A10" s="57" t="s">
+    <row r="10" s="18" customFormat="1" ht="85.5">
+      <c r="A10" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="83" t="s">
         <v>527</v>
       </c>
-      <c r="D10" s="90" t="s">
+      <c r="D10" s="83" t="s">
         <v>528</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="57" t="s">
         <v>529</v>
       </c>
       <c r="H10" s="18" t="s">
@@ -3909,40 +3878,40 @@
       </c>
     </row>
     <row r="11" s="18" customFormat="1" ht="57">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="55" t="s">
         <v>225</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="84" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="83" t="s">
         <v>513</v>
       </c>
-      <c r="D11" s="90" t="s">
+      <c r="D11" s="83" t="s">
         <v>530</v>
       </c>
-      <c r="E11" s="93" t="s">
+      <c r="E11" t="s">
         <v>378</v>
       </c>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="95"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" s="23" customFormat="1" ht="97.5" customHeight="1">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="59" t="s">
         <v>531</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>449</v>
-      </c>
-      <c r="C12" s="62" t="s">
+        <v>451</v>
+      </c>
+      <c r="C12" s="60" t="s">
         <v>532</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="60" t="s">
         <v>533</v>
       </c>
-      <c r="F12" s="96"/>
-      <c r="G12" s="63" t="s">
+      <c r="F12" s="85"/>
+      <c r="G12" s="61" t="s">
         <v>534</v>
       </c>
       <c r="H12" s="18" t="s">
@@ -3950,23 +3919,23 @@
       </c>
     </row>
     <row r="13" s="23" customFormat="1" ht="42.75">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="59" t="s">
         <v>535</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>536</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="60" t="s">
         <v>537</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="60" t="s">
         <v>538</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63" t="s">
+      <c r="F13" s="61"/>
+      <c r="G13" s="61" t="s">
         <v>539</v>
       </c>
       <c r="H13" s="18" t="s">
@@ -3974,20 +3943,20 @@
       </c>
     </row>
     <row r="14" s="23" customFormat="1">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="59" t="s">
         <v>540</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>541</v>
       </c>
-      <c r="C14" s="62" t="s">
+      <c r="C14" s="60" t="s">
         <v>542</v>
       </c>
-      <c r="D14" s="62" t="s">
+      <c r="D14" s="60" t="s">
         <v>543</v>
       </c>
-      <c r="F14" s="63"/>
-      <c r="G14" s="97" t="s">
+      <c r="F14" s="61"/>
+      <c r="G14" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H14" s="23" t="s">
@@ -3995,20 +3964,20 @@
       </c>
     </row>
     <row r="15" s="23" customFormat="1" ht="28.5">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="59" t="s">
         <v>545</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="60" t="s">
         <v>546</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="60" t="s">
         <v>547</v>
       </c>
-      <c r="F15" s="63"/>
-      <c r="G15" s="97" t="s">
+      <c r="F15" s="61"/>
+      <c r="G15" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H15" s="23" t="s">
@@ -4016,20 +3985,20 @@
       </c>
     </row>
     <row r="16" s="23" customFormat="1" ht="42.75">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="59" t="s">
         <v>548</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>549</v>
       </c>
-      <c r="C16" s="62" t="s">
+      <c r="C16" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="60" t="s">
         <v>550</v>
       </c>
-      <c r="F16" s="63"/>
-      <c r="G16" s="97" t="s">
+      <c r="F16" s="61"/>
+      <c r="G16" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H16" s="23" t="s">
@@ -4037,20 +4006,20 @@
       </c>
     </row>
     <row r="17" s="23" customFormat="1" ht="28.5">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="59" t="s">
         <v>551</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>552</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="60" t="s">
         <v>553</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="60" t="s">
         <v>554</v>
       </c>
-      <c r="F17" s="63"/>
-      <c r="G17" s="97" t="s">
+      <c r="F17" s="61"/>
+      <c r="G17" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H17" s="23" t="s">
@@ -4058,20 +4027,20 @@
       </c>
     </row>
     <row r="18" s="23" customFormat="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="59" t="s">
         <v>555</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>556</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="62" t="s">
+      <c r="D18" s="60" t="s">
         <v>557</v>
       </c>
-      <c r="F18" s="63"/>
-      <c r="G18" s="97" t="s">
+      <c r="F18" s="61"/>
+      <c r="G18" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H18" s="23" t="s">
@@ -4079,20 +4048,20 @@
       </c>
     </row>
     <row r="19" s="23" customFormat="1">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="59" t="s">
         <v>558</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="60" t="s">
         <v>559</v>
       </c>
-      <c r="F19" s="63"/>
-      <c r="G19" s="97" t="s">
+      <c r="F19" s="61"/>
+      <c r="G19" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H19" s="23" t="s">
@@ -4100,20 +4069,20 @@
       </c>
     </row>
     <row r="20" s="23" customFormat="1">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="59" t="s">
         <v>560</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>561</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="62" t="s">
+      <c r="D20" s="60" t="s">
         <v>562</v>
       </c>
-      <c r="F20" s="63"/>
-      <c r="G20" s="97" t="s">
+      <c r="F20" s="61"/>
+      <c r="G20" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H20" s="23" t="s">
@@ -4121,49 +4090,49 @@
       </c>
     </row>
     <row r="21" s="23" customFormat="1">
-      <c r="A21" s="61" t="s">
+      <c r="A21" s="59" t="s">
         <v>563</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>564</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="60" t="s">
         <v>565</v>
       </c>
-      <c r="F21" s="63"/>
-      <c r="G21" s="97" t="s">
+      <c r="F21" s="61"/>
+      <c r="G21" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H21" s="23" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="22" s="98" customFormat="1" ht="28.5">
-      <c r="A22" s="99" t="s">
+    <row r="22" s="87" customFormat="1" ht="28.5">
+      <c r="A22" s="88" t="s">
         <v>566</v>
       </c>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="87" t="s">
         <v>567</v>
       </c>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="89" t="s">
         <v>568</v>
       </c>
-      <c r="D22" s="100" t="s">
+      <c r="D22" s="89" t="s">
         <v>569</v>
       </c>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102" t="s">
+      <c r="F22" s="90"/>
+      <c r="G22" s="91" t="s">
         <v>544</v>
       </c>
-      <c r="H22" s="98" t="s">
+      <c r="H22" s="87" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="26" s="5" customFormat="1">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -4175,7 +4144,7 @@
       <c r="G26" s="9"/>
     </row>
     <row r="27" s="5" customFormat="1">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -4187,10 +4156,10 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" s="5" customFormat="1">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="103" t="s">
+      <c r="B28" s="92" t="s">
         <v>571</v>
       </c>
       <c r="C28" s="8"/>
@@ -4198,50 +4167,50 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="30" s="104" customFormat="1">
-      <c r="A30" s="104" t="s">
+    <row r="30" s="93" customFormat="1">
+      <c r="A30" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="104" t="s">
+      <c r="B30" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="105" t="s">
+      <c r="C30" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="105" t="s">
+      <c r="D30" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="104" t="s">
+      <c r="E30" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="106" t="s">
+      <c r="F30" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="106" t="s">
+      <c r="G30" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="104" t="s">
+      <c r="H30" s="93" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="31" s="18" customFormat="1">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="55" t="s">
         <v>560</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>561</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D31" s="56" t="s">
         <v>572</v>
       </c>
-      <c r="E31" s="107" t="s">
+      <c r="E31" s="96" t="s">
         <v>390</v>
       </c>
-      <c r="F31" s="59"/>
-      <c r="G31" s="108" t="s">
+      <c r="F31" s="57"/>
+      <c r="G31" s="97" t="s">
         <v>544</v>
       </c>
       <c r="H31" s="18" t="s">
@@ -4249,23 +4218,23 @@
       </c>
     </row>
     <row r="32" s="23" customFormat="1" ht="42.75">
-      <c r="A32" s="61" t="s">
+      <c r="A32" s="59" t="s">
         <v>573</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>574</v>
       </c>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="100" t="s">
+      <c r="D32" s="89" t="s">
         <v>575</v>
       </c>
-      <c r="E32" s="109" t="s">
+      <c r="E32" s="98" t="s">
         <v>378</v>
       </c>
-      <c r="F32" s="63"/>
-      <c r="G32" s="97" t="s">
+      <c r="F32" s="61"/>
+      <c r="G32" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H32" s="23" t="s">
@@ -4273,23 +4242,23 @@
       </c>
     </row>
     <row r="33" s="23" customFormat="1" ht="28.5">
-      <c r="A33" s="61" t="s">
+      <c r="A33" s="59" t="s">
         <v>253</v>
       </c>
       <c r="B33" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="C33" s="62" t="s">
+      <c r="C33" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="62" t="s">
+      <c r="D33" s="60" t="s">
         <v>576</v>
       </c>
-      <c r="E33" s="109" t="s">
+      <c r="E33" s="98" t="s">
         <v>390</v>
       </c>
-      <c r="F33" s="63"/>
-      <c r="G33" s="97" t="s">
+      <c r="F33" s="61"/>
+      <c r="G33" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H33" s="23" t="s">
@@ -4297,23 +4266,23 @@
       </c>
     </row>
     <row r="34" s="23" customFormat="1" ht="28.5">
-      <c r="A34" s="61" t="s">
+      <c r="A34" s="59" t="s">
         <v>555</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>556</v>
       </c>
-      <c r="C34" s="62" t="s">
+      <c r="C34" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="62" t="s">
+      <c r="D34" s="60" t="s">
         <v>577</v>
       </c>
-      <c r="E34" s="109" t="s">
+      <c r="E34" s="98" t="s">
         <v>578</v>
       </c>
-      <c r="F34" s="63"/>
-      <c r="G34" s="97" t="s">
+      <c r="F34" s="61"/>
+      <c r="G34" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H34" s="23" t="s">
@@ -4321,23 +4290,23 @@
       </c>
     </row>
     <row r="35" s="23" customFormat="1">
-      <c r="A35" s="61" t="s">
+      <c r="A35" s="59" t="s">
         <v>579</v>
       </c>
       <c r="B35" s="23" t="s">
         <v>564</v>
       </c>
-      <c r="C35" s="62" t="s">
+      <c r="C35" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="62" t="s">
+      <c r="D35" s="60" t="s">
         <v>580</v>
       </c>
-      <c r="E35" s="109" t="s">
+      <c r="E35" s="98" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="63"/>
-      <c r="G35" s="97" t="s">
+      <c r="F35" s="61"/>
+      <c r="G35" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H35" s="23" t="s">
@@ -4345,7 +4314,7 @@
       </c>
     </row>
     <row r="39" s="5" customFormat="1">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -4357,7 +4326,7 @@
       <c r="G39" s="9"/>
     </row>
     <row r="40" s="5" customFormat="1">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B40" s="13" t="s">
@@ -4369,10 +4338,10 @@
       <c r="G40" s="9"/>
     </row>
     <row r="41" s="5" customFormat="1">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="103" t="s">
+      <c r="B41" s="92" t="s">
         <v>571</v>
       </c>
       <c r="C41" s="8"/>
@@ -4407,23 +4376,23 @@
       </c>
     </row>
     <row r="44" s="23" customFormat="1" ht="30">
-      <c r="A44" s="61" t="s">
+      <c r="A44" s="59" t="s">
         <v>551</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>582</v>
       </c>
-      <c r="C44" s="62" t="s">
+      <c r="C44" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="62" t="s">
+      <c r="D44" s="60" t="s">
         <v>583</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F44" s="63"/>
-      <c r="G44" s="97" t="s">
+      <c r="F44" s="61"/>
+      <c r="G44" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H44" s="23" t="s">
@@ -4431,50 +4400,50 @@
       </c>
     </row>
     <row r="45" s="23" customFormat="1">
-      <c r="A45" s="61" t="s">
+      <c r="A45" s="59" t="s">
         <v>584</v>
       </c>
       <c r="B45" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="C45" s="62" t="s">
+      <c r="C45" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="62" t="s">
+      <c r="D45" s="60" t="s">
         <v>586</v>
       </c>
       <c r="E45" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F45" s="63"/>
-      <c r="G45" s="97" t="s">
+      <c r="F45" s="61"/>
+      <c r="G45" s="86" t="s">
         <v>544</v>
       </c>
       <c r="H45" s="23" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="46" s="98" customFormat="1" ht="42.75">
-      <c r="A46" s="99" t="s">
+    <row r="46" s="87" customFormat="1" ht="42.75">
+      <c r="A46" s="88" t="s">
         <v>587</v>
       </c>
-      <c r="B46" s="98" t="s">
-        <v>473</v>
-      </c>
-      <c r="C46" s="100" t="s">
+      <c r="B46" s="87" t="s">
+        <v>475</v>
+      </c>
+      <c r="C46" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="100" t="s">
+      <c r="D46" s="89" t="s">
         <v>588</v>
       </c>
-      <c r="E46" s="98" t="s">
+      <c r="E46" s="87" t="s">
         <v>390</v>
       </c>
-      <c r="F46" s="101"/>
-      <c r="G46" s="102" t="s">
+      <c r="F46" s="90"/>
+      <c r="G46" s="91" t="s">
         <v>544</v>
       </c>
-      <c r="H46" s="98" t="s">
+      <c r="H46" s="87" t="s">
         <v>395</v>
       </c>
     </row>
@@ -4511,7 +4480,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -4519,7 +4488,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -4527,10 +4496,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="74" t="s">
         <v>591</v>
       </c>
     </row>
@@ -4561,25 +4530,25 @@
       </c>
     </row>
     <row r="6" s="18" customFormat="1" ht="28.5">
-      <c r="A6" s="57" t="s">
-        <v>491</v>
+      <c r="A6" s="55" t="s">
+        <v>493</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="56" t="s">
         <v>592</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="57" t="s">
         <v>593</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="57" t="s">
         <v>72</v>
       </c>
       <c r="H6" s="18" t="s">
@@ -4587,7 +4556,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -4595,7 +4564,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -4603,10 +4572,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="74" t="s">
         <v>595</v>
       </c>
     </row>
@@ -4634,7 +4603,7 @@
       </c>
     </row>
     <row r="14" s="18" customFormat="1" ht="28.5">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="55" t="s">
         <v>596</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -4643,16 +4612,16 @@
       <c r="C14" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="56" t="s">
         <v>598</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="57" t="s">
         <v>599</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="57" t="s">
         <v>107</v>
       </c>
       <c r="H14" s="18" t="s">
@@ -4660,23 +4629,23 @@
       </c>
     </row>
     <row r="15" s="23" customFormat="1" ht="28.5">
-      <c r="A15" s="61" t="s">
-        <v>491</v>
+      <c r="A15" s="59" t="s">
+        <v>493</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="60" t="s">
         <v>600</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63" t="s">
+      <c r="F15" s="61"/>
+      <c r="G15" s="61" t="s">
         <v>107</v>
       </c>
       <c r="H15" s="23" t="s">
@@ -4710,7 +4679,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -4718,7 +4687,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -4726,10 +4695,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>603</v>
       </c>
     </row>
@@ -4772,23 +4741,23 @@
       </c>
     </row>
     <row r="7" s="18" customFormat="1" ht="57">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="56" t="s">
         <v>604</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>605</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -4796,23 +4765,23 @@
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="59" t="s">
         <v>271</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>606</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="60" t="s">
         <v>607</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="60" t="s">
         <v>608</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>609</v>
       </c>
-      <c r="F8" s="96"/>
-      <c r="G8" s="63" t="s">
+      <c r="F8" s="85"/>
+      <c r="G8" s="61" t="s">
         <v>610</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -5004,7 +4973,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -5015,7 +4984,7 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -5026,10 +4995,10 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="99" t="s">
         <v>571</v>
       </c>
       <c r="C3" s="8"/>
@@ -5068,25 +5037,25 @@
       </c>
     </row>
     <row r="6" ht="42.75">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="55" t="s">
         <v>613</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>614</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="111" t="s">
+      <c r="D6" s="100" t="s">
         <v>615</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="F6" s="56" t="s">
         <v>616</v>
       </c>
-      <c r="G6" s="59" t="s">
+      <c r="G6" s="57" t="s">
         <v>617</v>
       </c>
       <c r="H6" s="18" t="s">
@@ -5094,25 +5063,25 @@
       </c>
     </row>
     <row r="7" ht="128.25" customHeight="1">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>618</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>619</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="111" t="s">
+      <c r="D7" s="100" t="s">
         <v>620</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="F7" s="58" t="s">
+      <c r="F7" s="56" t="s">
         <v>621</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="57" t="s">
         <v>622</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -5120,25 +5089,25 @@
       </c>
     </row>
     <row r="8" ht="42.75">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="55" t="s">
         <v>623</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>624</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="111" t="s">
+      <c r="D8" s="100" t="s">
         <v>625</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="56" t="s">
         <v>626</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="57" t="s">
         <v>627</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -5146,25 +5115,25 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="59" t="s">
         <v>628</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>629</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="60" t="s">
         <v>376</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="60" t="s">
         <v>630</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="56" t="s">
         <v>631</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="57" t="s">
         <v>632</v>
       </c>
       <c r="H9" s="18" t="s">
@@ -5172,25 +5141,25 @@
       </c>
     </row>
     <row r="10" ht="28.5">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="59" t="s">
         <v>633</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>634</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="60" t="s">
         <v>635</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="60" t="s">
         <v>636</v>
       </c>
-      <c r="G10" s="63" t="s">
+      <c r="G10" s="61" t="s">
         <v>637</v>
       </c>
       <c r="H10" s="18" t="s">
@@ -5198,16 +5167,16 @@
       </c>
     </row>
     <row r="11" ht="57">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="101" t="s">
         <v>638</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="31" t="s">
         <v>639</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>640</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -5221,7 +5190,7 @@
       </c>
     </row>
     <row r="12" ht="28.5">
-      <c r="A12" s="112" t="s">
+      <c r="A12" s="101" t="s">
         <v>642</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -5230,7 +5199,7 @@
       <c r="C12" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>644</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -5244,7 +5213,7 @@
       </c>
     </row>
     <row r="13" ht="28.5">
-      <c r="A13" s="112" t="s">
+      <c r="A13" s="101" t="s">
         <v>646</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -5253,7 +5222,7 @@
       <c r="C13" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="31" t="s">
         <v>649</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -5262,13 +5231,13 @@
       <c r="F13" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="G13" s="113"/>
+      <c r="G13" s="102"/>
       <c r="H13" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="14" ht="28.5">
-      <c r="A14" s="112" t="s">
+      <c r="A14" s="101" t="s">
         <v>651</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -5277,7 +5246,7 @@
       <c r="C14" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="31" t="s">
         <v>652</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -5286,8 +5255,8 @@
       <c r="F14" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="G14" s="113"/>
-      <c r="H14" s="113" t="s">
+      <c r="G14" s="102"/>
+      <c r="H14" s="102" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5296,7 +5265,7 @@
       <c r="B15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -5307,10 +5276,10 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="46" t="s">
+      <c r="A17" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="114" t="s">
+      <c r="B17" s="103" t="s">
         <v>656</v>
       </c>
       <c r="C17" s="8"/>
@@ -5318,10 +5287,10 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="115" t="s">
+      <c r="B18" s="104" t="s">
         <v>571</v>
       </c>
       <c r="C18" s="8"/>
@@ -5358,23 +5327,23 @@
       </c>
     </row>
     <row r="21" ht="28.5">
-      <c r="A21" s="57" t="s">
+      <c r="A21" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="56" t="s">
         <v>657</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="58"/>
-      <c r="G21" s="59" t="s">
+      <c r="F21" s="56"/>
+      <c r="G21" s="57" t="s">
         <v>658</v>
       </c>
       <c r="H21" s="18" t="s">
@@ -5382,7 +5351,7 @@
       </c>
     </row>
     <row r="22" ht="28.5">
-      <c r="A22" s="61" t="s">
+      <c r="A22" s="59" t="s">
         <v>263</v>
       </c>
       <c r="B22" s="23" t="s">
@@ -5391,13 +5360,13 @@
       <c r="C22" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="62" t="s">
+      <c r="D22" s="60" t="s">
         <v>659</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="62"/>
+      <c r="F22" s="60"/>
       <c r="G22" s="23" t="s">
         <v>660</v>
       </c>
@@ -5406,7 +5375,7 @@
       </c>
     </row>
     <row r="23" ht="57">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="70" t="s">
         <v>132</v>
       </c>
       <c r="B23" t="s">
@@ -5430,7 +5399,7 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -5438,27 +5407,27 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="116"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="113"/>
+      <c r="H26" s="102"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="46" t="s">
+      <c r="A27" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="106" t="s">
         <v>648</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="116"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="113"/>
+      <c r="H27" s="102"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5466,20 +5435,20 @@
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="116"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="105"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="113"/>
+      <c r="H28" s="102"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="113"/>
-      <c r="B29" s="113"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="102"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="116"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="105"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="113"/>
+      <c r="H29" s="102"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="4" t="s">
@@ -5506,23 +5475,23 @@
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D31" s="56" t="s">
         <v>666</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="58"/>
-      <c r="G31" s="59" t="s">
+      <c r="F31" s="56"/>
+      <c r="G31" s="57" t="s">
         <v>667</v>
       </c>
       <c r="H31" s="18" t="s">
@@ -5530,23 +5499,23 @@
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="55" t="s">
         <v>144</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>549</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C32" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="56" t="s">
         <v>668</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="58"/>
-      <c r="G32" s="59" t="s">
+      <c r="F32" s="56"/>
+      <c r="G32" s="57" t="s">
         <v>669</v>
       </c>
       <c r="H32" s="18" t="s">
@@ -5555,56 +5524,56 @@
     </row>
     <row r="33" ht="14.25"/>
     <row r="35" ht="14.25">
-      <c r="A35" s="118" t="s">
+      <c r="A35" s="107" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="119" t="s">
+      <c r="B35" s="108" t="s">
         <v>670</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="116"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="105"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="113"/>
+      <c r="H35" s="102"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="120" t="s">
+      <c r="A36" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="121" t="s">
+      <c r="B36" s="110" t="s">
         <v>612</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="113"/>
-      <c r="F36" s="116"/>
+      <c r="E36" s="102"/>
+      <c r="F36" s="105"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="113"/>
+      <c r="H36" s="102"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="122" t="s">
+      <c r="A37" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="123" t="s">
+      <c r="B37" s="112" t="s">
         <v>671</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="116"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="105"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="113"/>
+      <c r="H37" s="102"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="113"/>
-      <c r="B38" s="113"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="113"/>
-      <c r="F38" s="116"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="105"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="113"/>
+      <c r="H38" s="102"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="4" t="s">
@@ -5631,23 +5600,23 @@
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="57" t="s">
+      <c r="A40" s="55" t="s">
         <v>253</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C40" s="58" t="s">
+      <c r="C40" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="56" t="s">
         <v>672</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="58"/>
-      <c r="G40" s="59" t="s">
+      <c r="F40" s="56"/>
+      <c r="G40" s="57" t="s">
         <v>673</v>
       </c>
       <c r="H40" s="18" t="s">
@@ -5655,7 +5624,7 @@
       </c>
     </row>
     <row r="41" ht="28.5">
-      <c r="A41" s="112" t="s">
+      <c r="A41" s="101" t="s">
         <v>646</v>
       </c>
       <c r="B41" t="s">
@@ -5664,15 +5633,15 @@
       <c r="C41" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="D41" s="31" t="s">
         <v>649</v>
       </c>
       <c r="E41" t="s">
         <v>609</v>
       </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="113"/>
-      <c r="H41" s="113" t="s">
+      <c r="G41" s="102"/>
+      <c r="H41" s="102" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5703,7 +5672,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="113" t="s">
         <v>674</v>
       </c>
       <c r="B1" t="s">
@@ -5711,7 +5680,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="113" t="s">
         <v>676</v>
       </c>
       <c r="B2" t="s">
@@ -5719,7 +5688,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="114" t="s">
         <v>678</v>
       </c>
     </row>
@@ -5811,15 +5780,15 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="113" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="113" t="s">
         <v>676</v>
       </c>
       <c r="B2" t="s">
@@ -5827,7 +5796,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="114" t="s">
         <v>678</v>
       </c>
     </row>
@@ -5895,15 +5864,15 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="113" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="113" t="s">
         <v>676</v>
       </c>
       <c r="B2" t="s">
@@ -5911,7 +5880,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="114" t="s">
         <v>678</v>
       </c>
     </row>
@@ -6174,10 +6143,10 @@
       </c>
     </row>
     <row r="12" s="23" customFormat="1" ht="28.5">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="28" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -6213,7 +6182,7 @@
       <c r="E13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="29" t="s">
         <v>100</v>
       </c>
       <c r="G13" s="27" t="s">
@@ -6239,7 +6208,7 @@
       <c r="E14" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="30" t="s">
         <v>106</v>
       </c>
       <c r="G14" s="27" t="s">
@@ -6259,7 +6228,7 @@
       <c r="C15" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="31" t="s">
         <v>110</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -6313,7 +6282,7 @@
       <c r="E17" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="29" t="s">
         <v>122</v>
       </c>
       <c r="G17" s="27" t="s">
@@ -6393,7 +6362,7 @@
       <c r="G20" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6413,16 +6382,16 @@
       <c r="E21" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="29" t="s">
         <v>142</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="I21" s="34"/>
+      <c r="I21" s="23"/>
     </row>
     <row r="22" s="23" customFormat="1" ht="28.5">
       <c r="A22" s="24" t="s">
@@ -6446,7 +6415,7 @@
       <c r="G22" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6466,7 +6435,7 @@
       <c r="E23" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="29" t="s">
         <v>150</v>
       </c>
       <c r="G23" s="27" t="s">
@@ -6483,7 +6452,7 @@
       <c r="B24" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="33" t="s">
         <v>154</v>
       </c>
       <c r="D24" s="26" t="s">
@@ -6498,7 +6467,7 @@
       <c r="G24" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6518,7 +6487,7 @@
       <c r="E25" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="29" t="s">
         <v>163</v>
       </c>
       <c r="G25" s="27" t="s">
@@ -6548,7 +6517,7 @@
       <c r="G26" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6572,7 +6541,7 @@
       <c r="G27" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6592,7 +6561,7 @@
       <c r="E28" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="29" t="s">
         <v>177</v>
       </c>
       <c r="G28" s="27" t="s">
@@ -6644,7 +6613,7 @@
       <c r="E30" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="30" t="s">
+      <c r="F30" s="29" t="s">
         <v>189</v>
       </c>
       <c r="G30" s="27" t="s">
@@ -6670,7 +6639,7 @@
       <c r="E31" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="29" t="s">
         <v>195</v>
       </c>
       <c r="G31" s="27" t="s">
@@ -6714,7 +6683,7 @@
       <c r="C33" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="34" t="s">
         <v>203</v>
       </c>
       <c r="E33" s="25" t="s">
@@ -6762,7 +6731,7 @@
       <c r="C35" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="35" t="s">
         <v>211</v>
       </c>
       <c r="E35" s="25" t="s">
@@ -6792,7 +6761,7 @@
       <c r="E36" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="30" t="s">
+      <c r="F36" s="29" t="s">
         <v>217</v>
       </c>
       <c r="G36" s="27" t="s">
@@ -6818,7 +6787,7 @@
       <c r="E37" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F37" s="29" t="s">
         <v>223</v>
       </c>
       <c r="G37" s="27" t="s">
@@ -6909,7 +6878,7 @@
       <c r="B41" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="36" t="s">
         <v>240</v>
       </c>
       <c r="D41" s="26" t="s">
@@ -6946,7 +6915,7 @@
       <c r="G42" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="H42" s="33" t="s">
+      <c r="H42" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6972,7 +6941,7 @@
       <c r="G43" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="H43" s="33" t="s">
+      <c r="H43" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6992,7 +6961,7 @@
       <c r="E44" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="30"/>
+      <c r="F44" s="29"/>
       <c r="G44" s="27" t="s">
         <v>252</v>
       </c>
@@ -7020,7 +6989,7 @@
       <c r="G45" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="H45" s="33" t="s">
+      <c r="H45" s="32" t="s">
         <v>137</v>
       </c>
     </row>
@@ -7044,7 +7013,7 @@
       <c r="G46" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="H46" s="39" t="s">
+      <c r="H46" s="37" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7118,18 +7087,18 @@
       <c r="G49" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H49" s="33" t="s">
+      <c r="H49" s="32" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="50" ht="57">
-      <c r="A50" s="40" t="s">
+      <c r="A50" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="B50" s="41" t="s">
+      <c r="B50" s="39" t="s">
         <v>276</v>
       </c>
-      <c r="C50" s="36" t="s">
+      <c r="C50" s="34" t="s">
         <v>277</v>
       </c>
       <c r="D50" s="8" t="s">
@@ -7218,7 +7187,7 @@
       <c r="C3" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -7238,7 +7207,7 @@
       <c r="C4" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -7258,7 +7227,7 @@
       <c r="C5" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E5" s="25" t="s">
@@ -7278,7 +7247,7 @@
       <c r="C6" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E6" s="25" t="s">
@@ -7298,7 +7267,7 @@
       <c r="C7" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="25" t="s">
@@ -7318,7 +7287,7 @@
       <c r="C8" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -7338,7 +7307,7 @@
       <c r="C9" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E9" s="25" t="s">
@@ -7358,7 +7327,7 @@
       <c r="C10" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E10" s="25" t="s">
@@ -7378,7 +7347,7 @@
       <c r="C11" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E11" s="25" t="s">
@@ -7418,7 +7387,7 @@
       <c r="C13" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E13" s="25" t="s">
@@ -7438,7 +7407,7 @@
       <c r="C14" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -7458,7 +7427,7 @@
       <c r="C15" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -7478,7 +7447,7 @@
       <c r="C16" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E16" s="25" t="s">
@@ -7498,7 +7467,7 @@
       <c r="C17" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E17" s="25" t="s">
@@ -7518,7 +7487,7 @@
       <c r="C18" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="42" t="s">
+      <c r="D18" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E18" s="25" t="s">
@@ -7558,7 +7527,7 @@
       <c r="C20" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -7578,7 +7547,7 @@
       <c r="C21" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="42" t="s">
+      <c r="D21" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E21" s="25" t="s">
@@ -7598,7 +7567,7 @@
       <c r="C22" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D22" s="42" t="s">
+      <c r="D22" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E22" s="25" t="s">
@@ -7618,7 +7587,7 @@
       <c r="C23" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E23" s="25" t="s">
@@ -7638,7 +7607,7 @@
       <c r="C24" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D24" s="42" t="s">
+      <c r="D24" s="40" t="s">
         <v>283</v>
       </c>
       <c r="E24" s="25" t="s">
@@ -7658,7 +7627,7 @@
       <c r="C25" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D25" s="42" t="s">
+      <c r="D25" s="40" t="s">
         <v>352</v>
       </c>
       <c r="E25" s="25" t="s">
@@ -7678,7 +7647,7 @@
       <c r="C26" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D26" s="42" t="s">
+      <c r="D26" s="40" t="s">
         <v>352</v>
       </c>
       <c r="E26" s="25" t="s">
@@ -7698,7 +7667,7 @@
       <c r="C27" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="41" t="s">
         <v>357</v>
       </c>
       <c r="E27" s="25" t="s">
@@ -7718,7 +7687,7 @@
       <c r="C28" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D28" s="43" t="s">
+      <c r="D28" s="41" t="s">
         <v>357</v>
       </c>
       <c r="E28" s="25" t="s">
@@ -7738,7 +7707,7 @@
       <c r="C29" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D29" s="43" t="s">
+      <c r="D29" s="41" t="s">
         <v>357</v>
       </c>
       <c r="E29" s="25" t="s">
@@ -7778,7 +7747,7 @@
       <c r="C31" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D31" s="43" t="s">
+      <c r="D31" s="41" t="s">
         <v>357</v>
       </c>
       <c r="E31" s="25" t="s">
@@ -7799,7 +7768,7 @@
       <c r="C32" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D32" s="43" t="s">
+      <c r="D32" s="41" t="s">
         <v>357</v>
       </c>
       <c r="E32" s="25" t="s">
@@ -7838,11 +7807,11 @@
     <col customWidth="1" min="4" max="4" style="8" width="50.5703125"/>
     <col customWidth="1" min="5" max="5" width="7.140625"/>
     <col customWidth="1" hidden="1" min="6" max="6" style="9" width="50.85546875"/>
-    <col customWidth="1" min="7" max="7" style="44" width="8"/>
+    <col customWidth="1" min="7" max="7" style="42" width="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -7850,7 +7819,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -7858,7 +7827,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -7884,55 +7853,55 @@
       <c r="F5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="46" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="6" s="49" customFormat="1" ht="28.5">
-      <c r="A6" s="50" t="s">
+    <row r="6" s="47" customFormat="1" ht="28.5">
+      <c r="A6" s="48" t="s">
         <v>374</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="49" t="s">
         <v>375</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="50" t="s">
         <v>376</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="50" t="s">
         <v>377</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="51" t="s">
         <v>378</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="55" t="s">
+      <c r="F6" s="52"/>
+      <c r="G6" s="53" t="s">
         <v>379</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="54" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="7" s="18" customFormat="1" ht="141" customHeight="1">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="55" t="s">
         <v>381</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="56" t="s">
         <v>383</v>
       </c>
-      <c r="D7" s="58" t="s">
+      <c r="D7" s="56" t="s">
         <v>384</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>385</v>
       </c>
-      <c r="F7" s="59"/>
-      <c r="G7" s="60" t="s">
+      <c r="F7" s="57"/>
+      <c r="G7" s="58" t="s">
         <v>386</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -7940,23 +7909,23 @@
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="42.75">
-      <c r="A8" s="61" t="s">
+      <c r="A8" s="59" t="s">
         <v>387</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="35" t="s">
         <v>389</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64" t="s">
+      <c r="F8" s="61"/>
+      <c r="G8" s="62" t="s">
         <v>386</v>
       </c>
       <c r="H8" s="23" t="s">
@@ -7989,11 +7958,11 @@
     <col customWidth="1" min="4" max="4" style="8" width="31.42578125"/>
     <col customWidth="1" min="5" max="5" width="6.85546875"/>
     <col customWidth="1" hidden="1" min="6" max="6" style="9" width="50.85546875"/>
-    <col customWidth="1" min="7" max="7" style="44" width="8.85546875"/>
+    <col customWidth="1" min="7" max="7" style="42" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8001,7 +7970,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8009,7 +7978,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -8035,7 +8004,7 @@
       <c r="F5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="46" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -8043,7 +8012,7 @@
       </c>
     </row>
     <row r="6" s="20" customFormat="1" ht="28.5">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="63" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -8059,39 +8028,39 @@
         <v>94</v>
       </c>
       <c r="F6" s="22"/>
-      <c r="G6" s="66" t="s">
+      <c r="G6" s="64" t="s">
         <v>247</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="H6" s="65" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="7" s="41" customFormat="1" ht="42.75">
-      <c r="A7" s="68" t="s">
+    <row r="7" s="39" customFormat="1" ht="42.75">
+      <c r="A7" s="66" t="s">
         <v>367</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="39" t="s">
         <v>396</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="39" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="34" t="s">
         <v>397</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70" t="s">
+      <c r="F7" s="67"/>
+      <c r="G7" s="68" t="s">
         <v>247</v>
       </c>
-      <c r="H7" s="71" t="s">
+      <c r="H7" s="69" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="72"/>
+      <c r="A8" s="70"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8118,12 +8087,12 @@
     <col customWidth="1" min="3" max="3" style="8" width="32.140625"/>
     <col customWidth="1" min="4" max="4" style="8" width="33.140625"/>
     <col customWidth="1" min="5" max="5" width="6"/>
-    <col customWidth="1" hidden="1" min="6" max="6" style="44" width="44.5703125"/>
+    <col customWidth="1" hidden="1" min="6" max="6" style="42" width="44.5703125"/>
     <col customWidth="1" min="7" max="7" style="9" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8131,7 +8100,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8139,7 +8108,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -8162,7 +8131,7 @@
       <c r="E5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="46" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="17" t="s">
@@ -8173,7 +8142,7 @@
       </c>
     </row>
     <row r="6" s="20" customFormat="1" ht="28.5">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="63" t="s">
         <v>400</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -8188,7 +8157,7 @@
       <c r="E6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="66" t="s">
+      <c r="F6" s="64" t="s">
         <v>403</v>
       </c>
       <c r="G6" s="22" t="s">
@@ -8199,7 +8168,7 @@
       </c>
     </row>
     <row r="7" s="25" customFormat="1" ht="57">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="71" t="s">
         <v>405</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -8214,18 +8183,18 @@
       <c r="E7" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>409</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H7" s="67" t="s">
+      <c r="H7" s="65" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="8" s="25" customFormat="1" ht="185.25">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="71" t="s">
         <v>411</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -8240,18 +8209,18 @@
       <c r="E8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="74" t="s">
+      <c r="F8" s="72" t="s">
         <v>414</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H8" s="67" t="s">
+      <c r="H8" s="65" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="9" s="25" customFormat="1" ht="85.5">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="71" t="s">
         <v>415</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -8266,13 +8235,13 @@
       <c r="E9" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="F9" s="74" t="s">
+      <c r="F9" s="72" t="s">
         <v>419</v>
       </c>
       <c r="G9" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="65" t="s">
         <v>395</v>
       </c>
     </row>
@@ -8304,13 +8273,13 @@
     <col customWidth="1" min="3" max="3" width="36.85546875"/>
     <col customWidth="1" min="4" max="4" style="8" width="38.85546875"/>
     <col customWidth="1" min="5" max="5" width="9.28515625"/>
-    <col customWidth="1" hidden="1" min="6" max="6" style="44" width="46.140625"/>
-    <col customWidth="1" min="7" max="7" style="44" width="19.5703125"/>
+    <col customWidth="1" hidden="1" min="6" max="6" style="42" width="46.140625"/>
+    <col customWidth="1" min="7" max="7" style="42" width="19.5703125"/>
     <col customWidth="1" min="8" max="8" width="12.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8318,7 +8287,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8326,42 +8295,42 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="73" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="74" t="s">
         <v>426</v>
       </c>
     </row>
@@ -8381,10 +8350,10 @@
       <c r="E9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="46" t="s">
         <v>58</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -8392,31 +8361,31 @@
       </c>
     </row>
     <row r="10" s="18" customFormat="1" ht="201.75" customHeight="1">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="55" t="s">
         <v>427</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="56" t="s">
         <v>429</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="56" t="s">
         <v>430</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="59" t="s">
+      <c r="F10" s="58"/>
+      <c r="G10" s="57" t="s">
         <v>431</v>
       </c>
-      <c r="H10" s="77" t="s">
+      <c r="H10" s="75" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="11" s="23" customFormat="1" ht="71.25">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="59" t="s">
         <v>433</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -8425,14 +8394,14 @@
       <c r="C11" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="60" t="s">
         <v>435</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64" t="s">
+      <c r="F11" s="62"/>
+      <c r="G11" s="62" t="s">
         <v>436</v>
       </c>
       <c r="H11" s="18" t="s">
@@ -8440,7 +8409,7 @@
       </c>
     </row>
     <row r="12" s="23" customFormat="1" ht="142.5">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="59" t="s">
         <v>437</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -8449,14 +8418,14 @@
       <c r="C12" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="D12" s="60" t="s">
         <v>439</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64" t="s">
+      <c r="F12" s="62"/>
+      <c r="G12" s="62" t="s">
         <v>440</v>
       </c>
       <c r="H12" s="18" t="s">
@@ -8496,7 +8465,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8504,7 +8473,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -8512,15 +8481,15 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="45" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -8554,78 +8523,78 @@
       </c>
     </row>
     <row r="7" s="18" customFormat="1" ht="57">
-      <c r="A7" s="57" t="s">
-        <v>90</v>
+      <c r="A7" s="55" t="s">
+        <v>445</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="58" t="s">
+        <v>446</v>
+      </c>
+      <c r="C7" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="58" t="s">
-        <v>445</v>
+      <c r="D7" s="56" t="s">
+        <v>447</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="59" t="s">
-        <v>446</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>447</v>
+      <c r="F7" s="57" t="s">
+        <v>448</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>449</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="71.25">
-      <c r="A8" s="61" t="s">
-        <v>448</v>
+      <c r="A8" s="59" t="s">
+        <v>450</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>449</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>450</v>
-      </c>
-      <c r="D8" s="62" t="s">
         <v>451</v>
+      </c>
+      <c r="C8" s="76" t="s">
+        <v>452</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>453</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="62" t="s">
-        <v>452</v>
-      </c>
-      <c r="G8" s="63" t="s">
-        <v>453</v>
+      <c r="F8" s="60" t="s">
+        <v>454</v>
+      </c>
+      <c r="G8" s="61" t="s">
+        <v>455</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="9" s="23" customFormat="1" ht="57">
-      <c r="A9" s="61" t="s">
-        <v>454</v>
+      <c r="A9" s="59" t="s">
+        <v>456</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>456</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>457</v>
+        <v>458</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>459</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="62" t="s">
-        <v>458</v>
-      </c>
-      <c r="G9" s="63" t="s">
-        <v>459</v>
+      <c r="F9" s="60" t="s">
+        <v>460</v>
+      </c>
+      <c r="G9" s="61" t="s">
+        <v>461</v>
       </c>
       <c r="H9" s="23" t="s">
         <v>380</v>
@@ -8638,44 +8607,44 @@
       <c r="G10" s="9"/>
     </row>
     <row r="11" s="5" customFormat="1">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="70" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D11" s="8"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" s="5" customFormat="1">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="70" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D12" s="8"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" s="5" customFormat="1">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="79" t="s">
-        <v>461</v>
+      <c r="B13" s="77" t="s">
+        <v>463</v>
       </c>
       <c r="D13" s="8"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
     </row>
     <row r="14" s="5" customFormat="1">
-      <c r="A14" s="72" t="s">
+      <c r="A14" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="79" t="s">
-        <v>462</v>
+      <c r="B14" s="77" t="s">
+        <v>464</v>
       </c>
       <c r="D14" s="8"/>
       <c r="F14" s="9"/>
@@ -8709,72 +8678,72 @@
       </c>
     </row>
     <row r="17" s="18" customFormat="1" ht="28.5">
-      <c r="A17" s="57" t="s">
-        <v>463</v>
+      <c r="A17" s="55" t="s">
+        <v>465</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>465</v>
-      </c>
-      <c r="D17" s="58" t="s">
-        <v>466</v>
+        <v>467</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>468</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59" t="s">
-        <v>467</v>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57" t="s">
+        <v>469</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="18" s="23" customFormat="1" ht="28.5">
-      <c r="A18" s="61" t="s">
-        <v>468</v>
+      <c r="A18" s="59" t="s">
+        <v>470</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>465</v>
-      </c>
-      <c r="D18" s="62" t="s">
-        <v>470</v>
+        <v>467</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>472</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63" t="s">
-        <v>471</v>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61" t="s">
+        <v>473</v>
       </c>
       <c r="H18" s="18" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="19" s="23" customFormat="1" ht="28.5">
-      <c r="A19" s="61" t="s">
-        <v>472</v>
+      <c r="A19" s="59" t="s">
+        <v>474</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>473</v>
-      </c>
-      <c r="C19" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="C19" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="62" t="s">
-        <v>474</v>
+      <c r="D19" s="60" t="s">
+        <v>476</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63" t="s">
-        <v>475</v>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61" t="s">
+        <v>477</v>
       </c>
       <c r="H19" s="18" t="s">
         <v>380</v>
@@ -8809,20 +8778,20 @@
     <col customWidth="1" min="3" max="3" width="26"/>
     <col customWidth="1" min="4" max="4" style="8" width="27.42578125"/>
     <col customWidth="1" min="5" max="5" width="9.7109375"/>
-    <col customWidth="1" hidden="1" min="6" max="6" style="44" width="46.140625"/>
-    <col customWidth="1" min="7" max="7" style="44" width="19.5703125"/>
+    <col customWidth="1" hidden="1" min="6" max="6" style="42" width="46.140625"/>
+    <col customWidth="1" min="7" max="7" style="42" width="19.5703125"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="43" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8830,11 +8799,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="76" t="s">
-        <v>477</v>
+      <c r="B3" s="74" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="5" s="4" customFormat="1">
@@ -8864,7 +8833,7 @@
       </c>
     </row>
     <row r="6" s="18" customFormat="1" ht="42.75">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="63" t="s">
         <v>263</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -8874,21 +8843,21 @@
         <v>129</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66" t="s">
-        <v>479</v>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64" t="s">
+        <v>481</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="7" s="23" customFormat="1" ht="42.75">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="71" t="s">
         <v>152</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -8898,21 +8867,21 @@
         <v>442</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80" t="s">
-        <v>481</v>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78" t="s">
+        <v>483</v>
       </c>
       <c r="H7" s="18" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="42.75">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="71" t="s">
         <v>257</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -8922,13 +8891,13 @@
         <v>259</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="80"/>
-      <c r="G8" s="80" t="s">
+      <c r="F8" s="78"/>
+      <c r="G8" s="78" t="s">
         <v>82</v>
       </c>
       <c r="H8" s="18" t="s">

</xml_diff>

<commit_message>
adjust record creation date
</commit_message>
<xml_diff>
--- a/application-profile-update/ISSN-Modele-v2.xlsx
+++ b/application-profile-update/ISSN-Modele-v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="10"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" state="visible" r:id="rId1"/>
@@ -2416,7 +2416,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="110">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2478,9 +2478,6 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="9" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
@@ -2607,19 +2604,9 @@
     <xf fontId="3" fillId="0" borderId="8" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3412,11 +3399,11 @@
     <col customWidth="1" min="4" max="4" style="8" width="36.85546875"/>
     <col customWidth="1" min="5" max="5" width="11.5703125"/>
     <col customWidth="1" hidden="1" min="6" max="6" style="9" width="53"/>
-    <col customWidth="1" min="7" max="7" style="42" width="13.28515625"/>
+    <col customWidth="1" min="7" max="7" style="41" width="13.28515625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -3424,7 +3411,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -3432,39 +3419,39 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="72" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="72" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -3498,16 +3485,16 @@
       </c>
     </row>
     <row r="10" s="18" customFormat="1" ht="57">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="62" t="s">
         <v>493</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>494</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="C10" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="80" t="s">
+      <c r="D10" s="21" t="s">
         <v>495</v>
       </c>
       <c r="E10" s="20" t="s">
@@ -3521,13 +3508,13 @@
       </c>
     </row>
     <row r="11" s="23" customFormat="1" ht="57">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="70" t="s">
         <v>415</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>416</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="78" t="s">
         <v>497</v>
       </c>
       <c r="D11" s="26" t="s">
@@ -3536,7 +3523,7 @@
       <c r="E11" s="25" t="s">
         <v>499</v>
       </c>
-      <c r="F11" s="81"/>
+      <c r="F11" s="79"/>
       <c r="G11" s="27" t="s">
         <v>500</v>
       </c>
@@ -3590,7 +3577,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -3598,7 +3585,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -3606,31 +3593,31 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="72" t="s">
         <v>490</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="72" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="20" s="4" customFormat="1">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="74" t="s">
+      <c r="B20" s="73" t="s">
         <v>512</v>
       </c>
       <c r="D20" s="8"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="42"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="4" t="s">
         <v>373</v>
       </c>
@@ -3638,7 +3625,7 @@
     <row r="21" s="18" customFormat="1">
       <c r="D21" s="8"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="42"/>
+      <c r="G21" s="41"/>
       <c r="H21" s="18" t="s">
         <v>380</v>
       </c>
@@ -3670,7 +3657,7 @@
       </c>
     </row>
     <row r="23" ht="128.25">
-      <c r="A23" s="63" t="s">
+      <c r="A23" s="62" t="s">
         <v>90</v>
       </c>
       <c r="B23" s="20" t="s">
@@ -3679,7 +3666,7 @@
       <c r="C23" s="20" t="s">
         <v>513</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="21" t="s">
         <v>514</v>
       </c>
       <c r="E23" s="20" t="s">
@@ -3691,7 +3678,7 @@
       </c>
     </row>
     <row r="24" ht="128.25">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="70" t="s">
         <v>515</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -3714,16 +3701,16 @@
       </c>
     </row>
     <row r="25" ht="14.25">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="70" t="s">
         <v>347</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="25" t="s">
         <v>520</v>
       </c>
-      <c r="D25" s="82" t="s">
+      <c r="D25" s="26" t="s">
         <v>521</v>
       </c>
       <c r="E25" s="25" t="s">
@@ -3770,7 +3757,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -3778,7 +3765,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -3786,34 +3773,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="72" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="6" s="5" customFormat="1">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="72" t="s">
         <v>526</v>
       </c>
       <c r="C6" s="8"/>
@@ -3854,23 +3841,23 @@
       </c>
     </row>
     <row r="10" s="18" customFormat="1" ht="85.5">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="54" t="s">
         <v>253</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="55" t="s">
         <v>527</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="55" t="s">
         <v>528</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57" t="s">
+      <c r="F10" s="56"/>
+      <c r="G10" s="56" t="s">
         <v>529</v>
       </c>
       <c r="H10" s="18" t="s">
@@ -3878,40 +3865,40 @@
       </c>
     </row>
     <row r="11" s="18" customFormat="1" ht="57">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="54" t="s">
         <v>225</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="55" t="s">
         <v>513</v>
       </c>
-      <c r="D11" s="83" t="s">
+      <c r="D11" s="55" t="s">
         <v>530</v>
       </c>
       <c r="E11" t="s">
         <v>378</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" s="23" customFormat="1" ht="97.5" customHeight="1">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="58" t="s">
         <v>531</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>451</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="59" t="s">
         <v>532</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="59" t="s">
         <v>533</v>
       </c>
-      <c r="F12" s="85"/>
-      <c r="G12" s="61" t="s">
+      <c r="F12" s="80"/>
+      <c r="G12" s="60" t="s">
         <v>534</v>
       </c>
       <c r="H12" s="18" t="s">
@@ -3919,23 +3906,23 @@
       </c>
     </row>
     <row r="13" s="23" customFormat="1" ht="42.75">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="58" t="s">
         <v>535</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>536</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="59" t="s">
         <v>537</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="59" t="s">
         <v>538</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61" t="s">
+      <c r="F13" s="60"/>
+      <c r="G13" s="60" t="s">
         <v>539</v>
       </c>
       <c r="H13" s="18" t="s">
@@ -3943,20 +3930,20 @@
       </c>
     </row>
     <row r="14" s="23" customFormat="1">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="58" t="s">
         <v>540</v>
       </c>
       <c r="B14" s="23" t="s">
         <v>541</v>
       </c>
-      <c r="C14" s="60" t="s">
+      <c r="C14" s="59" t="s">
         <v>542</v>
       </c>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="59" t="s">
         <v>543</v>
       </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="86" t="s">
+      <c r="F14" s="60"/>
+      <c r="G14" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H14" s="23" t="s">
@@ -3964,20 +3951,20 @@
       </c>
     </row>
     <row r="15" s="23" customFormat="1" ht="28.5">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="58" t="s">
         <v>545</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="59" t="s">
         <v>546</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="59" t="s">
         <v>547</v>
       </c>
-      <c r="F15" s="61"/>
-      <c r="G15" s="86" t="s">
+      <c r="F15" s="60"/>
+      <c r="G15" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H15" s="23" t="s">
@@ -3985,20 +3972,20 @@
       </c>
     </row>
     <row r="16" s="23" customFormat="1" ht="42.75">
-      <c r="A16" s="59" t="s">
+      <c r="A16" s="58" t="s">
         <v>548</v>
       </c>
       <c r="B16" s="23" t="s">
         <v>549</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="59" t="s">
         <v>550</v>
       </c>
-      <c r="F16" s="61"/>
-      <c r="G16" s="86" t="s">
+      <c r="F16" s="60"/>
+      <c r="G16" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H16" s="23" t="s">
@@ -4006,20 +3993,20 @@
       </c>
     </row>
     <row r="17" s="23" customFormat="1" ht="28.5">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="58" t="s">
         <v>551</v>
       </c>
       <c r="B17" s="23" t="s">
         <v>552</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="59" t="s">
         <v>553</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="59" t="s">
         <v>554</v>
       </c>
-      <c r="F17" s="61"/>
-      <c r="G17" s="86" t="s">
+      <c r="F17" s="60"/>
+      <c r="G17" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H17" s="23" t="s">
@@ -4027,20 +4014,20 @@
       </c>
     </row>
     <row r="18" s="23" customFormat="1">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="58" t="s">
         <v>555</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>556</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="59" t="s">
         <v>557</v>
       </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="86" t="s">
+      <c r="F18" s="60"/>
+      <c r="G18" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H18" s="23" t="s">
@@ -4048,20 +4035,20 @@
       </c>
     </row>
     <row r="19" s="23" customFormat="1">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="58" t="s">
         <v>558</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>559</v>
       </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="86" t="s">
+      <c r="F19" s="60"/>
+      <c r="G19" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H19" s="23" t="s">
@@ -4069,20 +4056,20 @@
       </c>
     </row>
     <row r="20" s="23" customFormat="1">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="58" t="s">
         <v>560</v>
       </c>
       <c r="B20" s="23" t="s">
         <v>561</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="59" t="s">
         <v>562</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="86" t="s">
+      <c r="F20" s="60"/>
+      <c r="G20" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H20" s="23" t="s">
@@ -4090,49 +4077,49 @@
       </c>
     </row>
     <row r="21" s="23" customFormat="1">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="58" t="s">
         <v>563</v>
       </c>
       <c r="B21" s="23" t="s">
         <v>564</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="59" t="s">
         <v>565</v>
       </c>
-      <c r="F21" s="61"/>
-      <c r="G21" s="86" t="s">
+      <c r="F21" s="60"/>
+      <c r="G21" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H21" s="23" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="22" s="87" customFormat="1" ht="28.5">
-      <c r="A22" s="88" t="s">
+    <row r="22" s="82" customFormat="1" ht="28.5">
+      <c r="A22" s="83" t="s">
         <v>566</v>
       </c>
-      <c r="B22" s="87" t="s">
+      <c r="B22" s="82" t="s">
         <v>567</v>
       </c>
-      <c r="C22" s="89" t="s">
+      <c r="C22" s="84" t="s">
         <v>568</v>
       </c>
-      <c r="D22" s="89" t="s">
+      <c r="D22" s="84" t="s">
         <v>569</v>
       </c>
-      <c r="F22" s="90"/>
-      <c r="G22" s="91" t="s">
+      <c r="F22" s="85"/>
+      <c r="G22" s="86" t="s">
         <v>544</v>
       </c>
-      <c r="H22" s="87" t="s">
+      <c r="H22" s="82" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="26" s="5" customFormat="1">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -4144,7 +4131,7 @@
       <c r="G26" s="9"/>
     </row>
     <row r="27" s="5" customFormat="1">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -4156,10 +4143,10 @@
       <c r="G27" s="9"/>
     </row>
     <row r="28" s="5" customFormat="1">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="92" t="s">
+      <c r="B28" s="87" t="s">
         <v>571</v>
       </c>
       <c r="C28" s="8"/>
@@ -4167,50 +4154,50 @@
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="30" s="93" customFormat="1">
-      <c r="A30" s="93" t="s">
+    <row r="30" s="88" customFormat="1">
+      <c r="A30" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="93" t="s">
+      <c r="B30" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C30" s="94" t="s">
+      <c r="C30" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="94" t="s">
+      <c r="D30" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="93" t="s">
+      <c r="E30" s="88" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="95" t="s">
+      <c r="F30" s="90" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="95" t="s">
+      <c r="G30" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="H30" s="93" t="s">
+      <c r="H30" s="88" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="31" s="18" customFormat="1">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="54" t="s">
         <v>560</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>561</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="56" t="s">
+      <c r="D31" s="55" t="s">
         <v>572</v>
       </c>
-      <c r="E31" s="96" t="s">
+      <c r="E31" s="91" t="s">
         <v>390</v>
       </c>
-      <c r="F31" s="57"/>
-      <c r="G31" s="97" t="s">
+      <c r="F31" s="56"/>
+      <c r="G31" s="92" t="s">
         <v>544</v>
       </c>
       <c r="H31" s="18" t="s">
@@ -4218,23 +4205,23 @@
       </c>
     </row>
     <row r="32" s="23" customFormat="1" ht="42.75">
-      <c r="A32" s="59" t="s">
+      <c r="A32" s="58" t="s">
         <v>573</v>
       </c>
       <c r="B32" s="23" t="s">
         <v>574</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="89" t="s">
+      <c r="D32" s="84" t="s">
         <v>575</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="93" t="s">
         <v>378</v>
       </c>
-      <c r="F32" s="61"/>
-      <c r="G32" s="86" t="s">
+      <c r="F32" s="60"/>
+      <c r="G32" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H32" s="23" t="s">
@@ -4242,23 +4229,23 @@
       </c>
     </row>
     <row r="33" s="23" customFormat="1" ht="28.5">
-      <c r="A33" s="59" t="s">
+      <c r="A33" s="58" t="s">
         <v>253</v>
       </c>
       <c r="B33" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="C33" s="60" t="s">
+      <c r="C33" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="59" t="s">
         <v>576</v>
       </c>
-      <c r="E33" s="98" t="s">
+      <c r="E33" s="93" t="s">
         <v>390</v>
       </c>
-      <c r="F33" s="61"/>
-      <c r="G33" s="86" t="s">
+      <c r="F33" s="60"/>
+      <c r="G33" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H33" s="23" t="s">
@@ -4266,23 +4253,23 @@
       </c>
     </row>
     <row r="34" s="23" customFormat="1" ht="28.5">
-      <c r="A34" s="59" t="s">
+      <c r="A34" s="58" t="s">
         <v>555</v>
       </c>
       <c r="B34" s="23" t="s">
         <v>556</v>
       </c>
-      <c r="C34" s="60" t="s">
+      <c r="C34" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="60" t="s">
+      <c r="D34" s="59" t="s">
         <v>577</v>
       </c>
-      <c r="E34" s="98" t="s">
+      <c r="E34" s="93" t="s">
         <v>578</v>
       </c>
-      <c r="F34" s="61"/>
-      <c r="G34" s="86" t="s">
+      <c r="F34" s="60"/>
+      <c r="G34" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H34" s="23" t="s">
@@ -4290,23 +4277,23 @@
       </c>
     </row>
     <row r="35" s="23" customFormat="1">
-      <c r="A35" s="59" t="s">
+      <c r="A35" s="58" t="s">
         <v>579</v>
       </c>
       <c r="B35" s="23" t="s">
         <v>564</v>
       </c>
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="59" t="s">
         <v>580</v>
       </c>
-      <c r="E35" s="98" t="s">
+      <c r="E35" s="93" t="s">
         <v>378</v>
       </c>
-      <c r="F35" s="61"/>
-      <c r="G35" s="86" t="s">
+      <c r="F35" s="60"/>
+      <c r="G35" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H35" s="23" t="s">
@@ -4314,7 +4301,7 @@
       </c>
     </row>
     <row r="39" s="5" customFormat="1">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -4326,7 +4313,7 @@
       <c r="G39" s="9"/>
     </row>
     <row r="40" s="5" customFormat="1">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B40" s="13" t="s">
@@ -4338,10 +4325,10 @@
       <c r="G40" s="9"/>
     </row>
     <row r="41" s="5" customFormat="1">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="92" t="s">
+      <c r="B41" s="87" t="s">
         <v>571</v>
       </c>
       <c r="C41" s="8"/>
@@ -4376,23 +4363,23 @@
       </c>
     </row>
     <row r="44" s="23" customFormat="1" ht="30">
-      <c r="A44" s="59" t="s">
+      <c r="A44" s="58" t="s">
         <v>551</v>
       </c>
       <c r="B44" s="23" t="s">
         <v>582</v>
       </c>
-      <c r="C44" s="60" t="s">
+      <c r="C44" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="60" t="s">
+      <c r="D44" s="59" t="s">
         <v>583</v>
       </c>
       <c r="E44" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="86" t="s">
+      <c r="F44" s="60"/>
+      <c r="G44" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H44" s="23" t="s">
@@ -4400,50 +4387,50 @@
       </c>
     </row>
     <row r="45" s="23" customFormat="1">
-      <c r="A45" s="59" t="s">
+      <c r="A45" s="58" t="s">
         <v>584</v>
       </c>
       <c r="B45" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D45" s="60" t="s">
+      <c r="D45" s="59" t="s">
         <v>586</v>
       </c>
       <c r="E45" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F45" s="61"/>
-      <c r="G45" s="86" t="s">
+      <c r="F45" s="60"/>
+      <c r="G45" s="81" t="s">
         <v>544</v>
       </c>
       <c r="H45" s="23" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="46" s="87" customFormat="1" ht="42.75">
-      <c r="A46" s="88" t="s">
+    <row r="46" s="82" customFormat="1" ht="42.75">
+      <c r="A46" s="83" t="s">
         <v>587</v>
       </c>
-      <c r="B46" s="87" t="s">
+      <c r="B46" s="82" t="s">
         <v>475</v>
       </c>
-      <c r="C46" s="89" t="s">
+      <c r="C46" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="89" t="s">
+      <c r="D46" s="84" t="s">
         <v>588</v>
       </c>
-      <c r="E46" s="87" t="s">
+      <c r="E46" s="82" t="s">
         <v>390</v>
       </c>
-      <c r="F46" s="90"/>
-      <c r="G46" s="91" t="s">
+      <c r="F46" s="85"/>
+      <c r="G46" s="86" t="s">
         <v>544</v>
       </c>
-      <c r="H46" s="87" t="s">
+      <c r="H46" s="82" t="s">
         <v>395</v>
       </c>
     </row>
@@ -4480,7 +4467,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -4488,7 +4475,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -4496,10 +4483,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="73" t="s">
         <v>591</v>
       </c>
     </row>
@@ -4530,7 +4517,7 @@
       </c>
     </row>
     <row r="6" s="18" customFormat="1" ht="28.5">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>493</v>
       </c>
       <c r="B6" s="18" t="s">
@@ -4539,16 +4526,16 @@
       <c r="C6" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="D6" s="55" t="s">
         <v>592</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="56" t="s">
         <v>593</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="56" t="s">
         <v>72</v>
       </c>
       <c r="H6" s="18" t="s">
@@ -4556,7 +4543,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -4564,7 +4551,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -4572,10 +4559,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="73" t="s">
         <v>595</v>
       </c>
     </row>
@@ -4603,7 +4590,7 @@
       </c>
     </row>
     <row r="14" s="18" customFormat="1" ht="28.5">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="54" t="s">
         <v>596</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -4612,16 +4599,16 @@
       <c r="C14" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="55" t="s">
         <v>598</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F14" s="56" t="s">
         <v>599</v>
       </c>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="56" t="s">
         <v>107</v>
       </c>
       <c r="H14" s="18" t="s">
@@ -4629,7 +4616,7 @@
       </c>
     </row>
     <row r="15" s="23" customFormat="1" ht="28.5">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="58" t="s">
         <v>493</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -4638,14 +4625,14 @@
       <c r="C15" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="59" t="s">
         <v>600</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61" t="s">
+      <c r="F15" s="60"/>
+      <c r="G15" s="60" t="s">
         <v>107</v>
       </c>
       <c r="H15" s="23" t="s">
@@ -4679,7 +4666,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -4687,7 +4674,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -4695,10 +4682,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>603</v>
       </c>
     </row>
@@ -4741,23 +4728,23 @@
       </c>
     </row>
     <row r="7" s="18" customFormat="1" ht="57">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="54" t="s">
         <v>253</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="55" t="s">
         <v>604</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="F7" s="56"/>
+      <c r="G7" s="56" t="s">
         <v>605</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -4765,23 +4752,23 @@
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="58" t="s">
         <v>271</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>606</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="59" t="s">
         <v>607</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="59" t="s">
         <v>608</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>609</v>
       </c>
-      <c r="F8" s="85"/>
-      <c r="G8" s="61" t="s">
+      <c r="F8" s="80"/>
+      <c r="G8" s="60" t="s">
         <v>610</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -4973,7 +4960,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -4984,7 +4971,7 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -4995,10 +4982,10 @@
       <c r="G2" s="9"/>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="94" t="s">
         <v>571</v>
       </c>
       <c r="C3" s="8"/>
@@ -5037,25 +5024,25 @@
       </c>
     </row>
     <row r="6" ht="42.75">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="54" t="s">
         <v>613</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>614</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="95" t="s">
         <v>615</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="56" t="s">
+      <c r="F6" s="55" t="s">
         <v>616</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="56" t="s">
         <v>617</v>
       </c>
       <c r="H6" s="18" t="s">
@@ -5063,25 +5050,25 @@
       </c>
     </row>
     <row r="7" ht="128.25" customHeight="1">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="54" t="s">
         <v>618</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>619</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="95" t="s">
         <v>620</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="55" t="s">
         <v>621</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="56" t="s">
         <v>622</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -5089,25 +5076,25 @@
       </c>
     </row>
     <row r="8" ht="42.75">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="54" t="s">
         <v>623</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>624</v>
       </c>
-      <c r="C8" s="56" t="s">
+      <c r="C8" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="95" t="s">
         <v>625</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>378</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="55" t="s">
         <v>626</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="56" t="s">
         <v>627</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -5115,25 +5102,25 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="58" t="s">
         <v>628</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>629</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="59" t="s">
         <v>376</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="59" t="s">
         <v>630</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>631</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="56" t="s">
         <v>632</v>
       </c>
       <c r="H9" s="18" t="s">
@@ -5141,25 +5128,25 @@
       </c>
     </row>
     <row r="10" ht="28.5">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="58" t="s">
         <v>633</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>634</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="D10" s="59" t="s">
         <v>635</v>
       </c>
       <c r="E10" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="59" t="s">
         <v>636</v>
       </c>
-      <c r="G10" s="61" t="s">
+      <c r="G10" s="60" t="s">
         <v>637</v>
       </c>
       <c r="H10" s="18" t="s">
@@ -5167,16 +5154,16 @@
       </c>
     </row>
     <row r="11" ht="57">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="96" t="s">
         <v>638</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>639</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="30" t="s">
         <v>640</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -5190,7 +5177,7 @@
       </c>
     </row>
     <row r="12" ht="28.5">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="96" t="s">
         <v>642</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -5199,7 +5186,7 @@
       <c r="C12" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="30" t="s">
         <v>644</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -5213,7 +5200,7 @@
       </c>
     </row>
     <row r="13" ht="28.5">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="96" t="s">
         <v>646</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -5222,7 +5209,7 @@
       <c r="C13" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>649</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -5231,13 +5218,13 @@
       <c r="F13" s="8" t="s">
         <v>650</v>
       </c>
-      <c r="G13" s="102"/>
+      <c r="G13" s="97"/>
       <c r="H13" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="14" ht="28.5">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="96" t="s">
         <v>651</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -5246,7 +5233,7 @@
       <c r="C14" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>652</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -5255,8 +5242,8 @@
       <c r="F14" s="8" t="s">
         <v>654</v>
       </c>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102" t="s">
+      <c r="G14" s="97"/>
+      <c r="H14" s="97" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5265,7 +5252,7 @@
       <c r="B15" s="5"/>
     </row>
     <row r="16">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -5276,10 +5263,10 @@
       <c r="G16" s="9"/>
     </row>
     <row r="17">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="103" t="s">
+      <c r="B17" s="98" t="s">
         <v>656</v>
       </c>
       <c r="C17" s="8"/>
@@ -5287,10 +5274,10 @@
       <c r="G17" s="9"/>
     </row>
     <row r="18">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="99" t="s">
         <v>571</v>
       </c>
       <c r="C18" s="8"/>
@@ -5327,23 +5314,23 @@
       </c>
     </row>
     <row r="21" ht="28.5">
-      <c r="A21" s="55" t="s">
+      <c r="A21" s="54" t="s">
         <v>253</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="C21" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="D21" s="55" t="s">
         <v>657</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57" t="s">
+      <c r="F21" s="55"/>
+      <c r="G21" s="56" t="s">
         <v>658</v>
       </c>
       <c r="H21" s="18" t="s">
@@ -5351,7 +5338,7 @@
       </c>
     </row>
     <row r="22" ht="28.5">
-      <c r="A22" s="59" t="s">
+      <c r="A22" s="58" t="s">
         <v>263</v>
       </c>
       <c r="B22" s="23" t="s">
@@ -5360,13 +5347,13 @@
       <c r="C22" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="59" t="s">
         <v>659</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F22" s="60"/>
+      <c r="F22" s="59"/>
       <c r="G22" s="23" t="s">
         <v>660</v>
       </c>
@@ -5375,7 +5362,7 @@
       </c>
     </row>
     <row r="23" ht="57">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="69" t="s">
         <v>132</v>
       </c>
       <c r="B23" t="s">
@@ -5399,7 +5386,7 @@
       </c>
     </row>
     <row r="26" ht="14.25">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="11" t="s">
@@ -5407,27 +5394,27 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="102"/>
-      <c r="F26" s="105"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="100"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="102"/>
+      <c r="H26" s="97"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="101" t="s">
         <v>648</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="102"/>
-      <c r="F27" s="105"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="100"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="102"/>
+      <c r="H27" s="97"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -5435,20 +5422,20 @@
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="102"/>
-      <c r="F28" s="105"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="100"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="102"/>
+      <c r="H28" s="97"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="A29" s="102"/>
-      <c r="B29" s="102"/>
+      <c r="A29" s="97"/>
+      <c r="B29" s="97"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="102"/>
-      <c r="F29" s="105"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="100"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="102"/>
+      <c r="H29" s="97"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="4" t="s">
@@ -5475,23 +5462,23 @@
       </c>
     </row>
     <row r="31" ht="14.25">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="54" t="s">
         <v>253</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="56" t="s">
+      <c r="D31" s="55" t="s">
         <v>666</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="56"/>
-      <c r="G31" s="57" t="s">
+      <c r="F31" s="55"/>
+      <c r="G31" s="56" t="s">
         <v>667</v>
       </c>
       <c r="H31" s="18" t="s">
@@ -5499,23 +5486,23 @@
       </c>
     </row>
     <row r="32" ht="14.25">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="54" t="s">
         <v>144</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>549</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="55" t="s">
         <v>668</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="56"/>
-      <c r="G32" s="57" t="s">
+      <c r="F32" s="55"/>
+      <c r="G32" s="56" t="s">
         <v>669</v>
       </c>
       <c r="H32" s="18" t="s">
@@ -5524,56 +5511,56 @@
     </row>
     <row r="33" ht="14.25"/>
     <row r="35" ht="14.25">
-      <c r="A35" s="107" t="s">
+      <c r="A35" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="108" t="s">
+      <c r="B35" s="103" t="s">
         <v>670</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="105"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="100"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="102"/>
+      <c r="H35" s="97"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="110" t="s">
+      <c r="B36" s="105" t="s">
         <v>612</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="105"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="100"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="102"/>
+      <c r="H36" s="97"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="A37" s="111" t="s">
+      <c r="A37" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="112" t="s">
+      <c r="B37" s="107" t="s">
         <v>671</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="102"/>
-      <c r="F37" s="105"/>
+      <c r="E37" s="97"/>
+      <c r="F37" s="100"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="102"/>
+      <c r="H37" s="97"/>
     </row>
     <row r="38" ht="14.25">
-      <c r="A38" s="102"/>
-      <c r="B38" s="102"/>
+      <c r="A38" s="97"/>
+      <c r="B38" s="97"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="102"/>
-      <c r="F38" s="105"/>
+      <c r="E38" s="97"/>
+      <c r="F38" s="100"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="102"/>
+      <c r="H38" s="97"/>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" s="4" t="s">
@@ -5600,23 +5587,23 @@
       </c>
     </row>
     <row r="40" ht="14.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="54" t="s">
         <v>253</v>
       </c>
       <c r="B40" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="55" t="s">
         <v>672</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="56"/>
-      <c r="G40" s="57" t="s">
+      <c r="F40" s="55"/>
+      <c r="G40" s="56" t="s">
         <v>673</v>
       </c>
       <c r="H40" s="18" t="s">
@@ -5624,7 +5611,7 @@
       </c>
     </row>
     <row r="41" ht="28.5">
-      <c r="A41" s="101" t="s">
+      <c r="A41" s="96" t="s">
         <v>646</v>
       </c>
       <c r="B41" t="s">
@@ -5633,15 +5620,15 @@
       <c r="C41" s="8" t="s">
         <v>648</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="30" t="s">
         <v>649</v>
       </c>
       <c r="E41" t="s">
         <v>609</v>
       </c>
       <c r="F41" s="8"/>
-      <c r="G41" s="102"/>
-      <c r="H41" s="102" t="s">
+      <c r="G41" s="97"/>
+      <c r="H41" s="97" t="s">
         <v>395</v>
       </c>
     </row>
@@ -5672,7 +5659,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="108" t="s">
         <v>674</v>
       </c>
       <c r="B1" t="s">
@@ -5680,7 +5667,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="108" t="s">
         <v>676</v>
       </c>
       <c r="B2" t="s">
@@ -5688,7 +5675,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="109" t="s">
         <v>678</v>
       </c>
     </row>
@@ -5780,15 +5767,15 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="108" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="76" t="s">
         <v>686</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="108" t="s">
         <v>676</v>
       </c>
       <c r="B2" t="s">
@@ -5796,7 +5783,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="109" t="s">
         <v>678</v>
       </c>
     </row>
@@ -5864,15 +5851,15 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="108" t="s">
         <v>674</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="76" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="108" t="s">
         <v>676</v>
       </c>
       <c r="B2" t="s">
@@ -5880,7 +5867,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="109" t="s">
         <v>678</v>
       </c>
     </row>
@@ -6146,7 +6133,7 @@
       <c r="A12" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="25" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="26" t="s">
@@ -6182,7 +6169,7 @@
       <c r="E13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="28" t="s">
         <v>100</v>
       </c>
       <c r="G13" s="27" t="s">
@@ -6208,7 +6195,7 @@
       <c r="E14" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="29" t="s">
         <v>106</v>
       </c>
       <c r="G14" s="27" t="s">
@@ -6228,7 +6215,7 @@
       <c r="C15" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>110</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -6282,7 +6269,7 @@
       <c r="E17" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="28" t="s">
         <v>122</v>
       </c>
       <c r="G17" s="27" t="s">
@@ -6362,7 +6349,7 @@
       <c r="G20" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6382,13 +6369,13 @@
       <c r="E21" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="28" t="s">
         <v>142</v>
       </c>
       <c r="G21" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="H21" s="32" t="s">
+      <c r="H21" s="31" t="s">
         <v>137</v>
       </c>
       <c r="I21" s="23"/>
@@ -6415,7 +6402,7 @@
       <c r="G22" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6435,7 +6422,7 @@
       <c r="E23" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="28" t="s">
         <v>150</v>
       </c>
       <c r="G23" s="27" t="s">
@@ -6452,7 +6439,7 @@
       <c r="B24" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="32" t="s">
         <v>154</v>
       </c>
       <c r="D24" s="26" t="s">
@@ -6467,7 +6454,7 @@
       <c r="G24" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="H24" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6487,7 +6474,7 @@
       <c r="E25" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="28" t="s">
         <v>163</v>
       </c>
       <c r="G25" s="27" t="s">
@@ -6517,7 +6504,7 @@
       <c r="G26" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="H26" s="32" t="s">
+      <c r="H26" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6541,7 +6528,7 @@
       <c r="G27" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="H27" s="32" t="s">
+      <c r="H27" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6561,7 +6548,7 @@
       <c r="E28" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="28" t="s">
         <v>177</v>
       </c>
       <c r="G28" s="27" t="s">
@@ -6613,7 +6600,7 @@
       <c r="E30" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="F30" s="28" t="s">
         <v>189</v>
       </c>
       <c r="G30" s="27" t="s">
@@ -6639,7 +6626,7 @@
       <c r="E31" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F31" s="28" t="s">
         <v>195</v>
       </c>
       <c r="G31" s="27" t="s">
@@ -6683,7 +6670,7 @@
       <c r="C33" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="33" t="s">
         <v>203</v>
       </c>
       <c r="E33" s="25" t="s">
@@ -6731,7 +6718,7 @@
       <c r="C35" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="34" t="s">
         <v>211</v>
       </c>
       <c r="E35" s="25" t="s">
@@ -6761,7 +6748,7 @@
       <c r="E36" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="29" t="s">
+      <c r="F36" s="28" t="s">
         <v>217</v>
       </c>
       <c r="G36" s="27" t="s">
@@ -6787,7 +6774,7 @@
       <c r="E37" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F37" s="28" t="s">
         <v>223</v>
       </c>
       <c r="G37" s="27" t="s">
@@ -6878,7 +6865,7 @@
       <c r="B41" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="35" t="s">
         <v>240</v>
       </c>
       <c r="D41" s="26" t="s">
@@ -6915,7 +6902,7 @@
       <c r="G42" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="H42" s="32" t="s">
+      <c r="H42" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6941,7 +6928,7 @@
       <c r="G43" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="H43" s="32" t="s">
+      <c r="H43" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6961,7 +6948,7 @@
       <c r="E44" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F44" s="29"/>
+      <c r="F44" s="28"/>
       <c r="G44" s="27" t="s">
         <v>252</v>
       </c>
@@ -6989,7 +6976,7 @@
       <c r="G45" s="27" t="s">
         <v>256</v>
       </c>
-      <c r="H45" s="32" t="s">
+      <c r="H45" s="31" t="s">
         <v>137</v>
       </c>
     </row>
@@ -7013,7 +7000,7 @@
       <c r="G46" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="36" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7087,18 +7074,18 @@
       <c r="G49" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H49" s="32" t="s">
+      <c r="H49" s="31" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="50" ht="57">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="38" t="s">
         <v>276</v>
       </c>
-      <c r="C50" s="34" t="s">
+      <c r="C50" s="33" t="s">
         <v>277</v>
       </c>
       <c r="D50" s="8" t="s">
@@ -7187,7 +7174,7 @@
       <c r="C3" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E3" s="20" t="s">
@@ -7207,7 +7194,7 @@
       <c r="C4" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -7227,7 +7214,7 @@
       <c r="C5" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E5" s="25" t="s">
@@ -7247,7 +7234,7 @@
       <c r="C6" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E6" s="25" t="s">
@@ -7267,7 +7254,7 @@
       <c r="C7" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E7" s="25" t="s">
@@ -7287,7 +7274,7 @@
       <c r="C8" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E8" s="25" t="s">
@@ -7307,7 +7294,7 @@
       <c r="C9" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D9" s="40" t="s">
+      <c r="D9" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E9" s="25" t="s">
@@ -7327,7 +7314,7 @@
       <c r="C10" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E10" s="25" t="s">
@@ -7347,7 +7334,7 @@
       <c r="C11" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E11" s="25" t="s">
@@ -7387,7 +7374,7 @@
       <c r="C13" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E13" s="25" t="s">
@@ -7407,7 +7394,7 @@
       <c r="C14" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -7427,7 +7414,7 @@
       <c r="C15" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D15" s="40" t="s">
+      <c r="D15" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -7447,7 +7434,7 @@
       <c r="C16" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E16" s="25" t="s">
@@ -7467,7 +7454,7 @@
       <c r="C17" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E17" s="25" t="s">
@@ -7487,7 +7474,7 @@
       <c r="C18" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E18" s="25" t="s">
@@ -7527,7 +7514,7 @@
       <c r="C20" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -7547,7 +7534,7 @@
       <c r="C21" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E21" s="25" t="s">
@@ -7567,7 +7554,7 @@
       <c r="C22" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E22" s="25" t="s">
@@ -7587,7 +7574,7 @@
       <c r="C23" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E23" s="25" t="s">
@@ -7607,7 +7594,7 @@
       <c r="C24" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="39" t="s">
         <v>283</v>
       </c>
       <c r="E24" s="25" t="s">
@@ -7627,7 +7614,7 @@
       <c r="C25" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="39" t="s">
         <v>352</v>
       </c>
       <c r="E25" s="25" t="s">
@@ -7647,7 +7634,7 @@
       <c r="C26" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="39" t="s">
         <v>352</v>
       </c>
       <c r="E26" s="25" t="s">
@@ -7667,7 +7654,7 @@
       <c r="C27" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D27" s="41" t="s">
+      <c r="D27" s="40" t="s">
         <v>357</v>
       </c>
       <c r="E27" s="25" t="s">
@@ -7687,7 +7674,7 @@
       <c r="C28" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D28" s="41" t="s">
+      <c r="D28" s="40" t="s">
         <v>357</v>
       </c>
       <c r="E28" s="25" t="s">
@@ -7707,7 +7694,7 @@
       <c r="C29" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="40" t="s">
         <v>357</v>
       </c>
       <c r="E29" s="25" t="s">
@@ -7747,7 +7734,7 @@
       <c r="C31" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D31" s="40" t="s">
         <v>357</v>
       </c>
       <c r="E31" s="25" t="s">
@@ -7768,7 +7755,7 @@
       <c r="C32" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="D32" s="41" t="s">
+      <c r="D32" s="40" t="s">
         <v>357</v>
       </c>
       <c r="E32" s="25" t="s">
@@ -7807,11 +7794,11 @@
     <col customWidth="1" min="4" max="4" style="8" width="50.5703125"/>
     <col customWidth="1" min="5" max="5" width="7.140625"/>
     <col customWidth="1" hidden="1" min="6" max="6" style="9" width="50.85546875"/>
-    <col customWidth="1" min="7" max="7" style="42" width="8"/>
+    <col customWidth="1" min="7" max="7" style="41" width="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -7819,7 +7806,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -7827,7 +7814,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -7853,55 +7840,55 @@
       <c r="F5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="6" s="47" customFormat="1" ht="28.5">
-      <c r="A6" s="48" t="s">
+    <row r="6" s="46" customFormat="1" ht="28.5">
+      <c r="A6" s="47" t="s">
         <v>374</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>375</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="49" t="s">
         <v>376</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="49" t="s">
         <v>377</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="50" t="s">
         <v>378</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53" t="s">
+      <c r="F6" s="51"/>
+      <c r="G6" s="52" t="s">
         <v>379</v>
       </c>
-      <c r="H6" s="54" t="s">
+      <c r="H6" s="53" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="7" s="18" customFormat="1" ht="141" customHeight="1">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="54" t="s">
         <v>381</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>382</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>383</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="55" t="s">
         <v>384</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>385</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="58" t="s">
+      <c r="F7" s="56"/>
+      <c r="G7" s="57" t="s">
         <v>386</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -7909,23 +7896,23 @@
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="42.75">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="58" t="s">
         <v>387</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>389</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F8" s="61"/>
-      <c r="G8" s="62" t="s">
+      <c r="F8" s="60"/>
+      <c r="G8" s="61" t="s">
         <v>386</v>
       </c>
       <c r="H8" s="23" t="s">
@@ -7958,11 +7945,11 @@
     <col customWidth="1" min="4" max="4" style="8" width="31.42578125"/>
     <col customWidth="1" min="5" max="5" width="6.85546875"/>
     <col customWidth="1" hidden="1" min="6" max="6" style="9" width="50.85546875"/>
-    <col customWidth="1" min="7" max="7" style="42" width="8.85546875"/>
+    <col customWidth="1" min="7" max="7" style="41" width="8.85546875"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -7970,7 +7957,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -7978,7 +7965,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -8004,7 +7991,7 @@
       <c r="F5" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -8012,7 +7999,7 @@
       </c>
     </row>
     <row r="6" s="20" customFormat="1" ht="28.5">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="62" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -8028,39 +8015,39 @@
         <v>94</v>
       </c>
       <c r="F6" s="22"/>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="63" t="s">
         <v>247</v>
       </c>
-      <c r="H6" s="65" t="s">
+      <c r="H6" s="64" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="7" s="39" customFormat="1" ht="42.75">
-      <c r="A7" s="66" t="s">
+    <row r="7" s="38" customFormat="1" ht="42.75">
+      <c r="A7" s="65" t="s">
         <v>367</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="38" t="s">
         <v>396</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="33" t="s">
         <v>397</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="68" t="s">
+      <c r="F7" s="66"/>
+      <c r="G7" s="67" t="s">
         <v>247</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="68" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="70"/>
+      <c r="A8" s="69"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8087,12 +8074,12 @@
     <col customWidth="1" min="3" max="3" style="8" width="32.140625"/>
     <col customWidth="1" min="4" max="4" style="8" width="33.140625"/>
     <col customWidth="1" min="5" max="5" width="6"/>
-    <col customWidth="1" hidden="1" min="6" max="6" style="42" width="44.5703125"/>
+    <col customWidth="1" hidden="1" min="6" max="6" style="41" width="44.5703125"/>
     <col customWidth="1" min="7" max="7" style="9" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8100,7 +8087,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8108,7 +8095,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -8131,7 +8118,7 @@
       <c r="E5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="45" t="s">
         <v>57</v>
       </c>
       <c r="G5" s="17" t="s">
@@ -8142,7 +8129,7 @@
       </c>
     </row>
     <row r="6" s="20" customFormat="1" ht="28.5">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="62" t="s">
         <v>400</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -8157,7 +8144,7 @@
       <c r="E6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="63" t="s">
         <v>403</v>
       </c>
       <c r="G6" s="22" t="s">
@@ -8168,7 +8155,7 @@
       </c>
     </row>
     <row r="7" s="25" customFormat="1" ht="57">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="70" t="s">
         <v>405</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -8183,18 +8170,18 @@
       <c r="E7" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>409</v>
       </c>
       <c r="G7" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H7" s="65" t="s">
+      <c r="H7" s="64" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="8" s="25" customFormat="1" ht="185.25">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="70" t="s">
         <v>411</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -8209,18 +8196,18 @@
       <c r="E8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="71" t="s">
         <v>414</v>
       </c>
       <c r="G8" s="27" t="s">
         <v>410</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="64" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="9" s="25" customFormat="1" ht="85.5">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="70" t="s">
         <v>415</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -8235,13 +8222,13 @@
       <c r="E9" s="25" t="s">
         <v>390</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="F9" s="71" t="s">
         <v>419</v>
       </c>
       <c r="G9" s="27" t="s">
         <v>420</v>
       </c>
-      <c r="H9" s="65" t="s">
+      <c r="H9" s="64" t="s">
         <v>395</v>
       </c>
     </row>
@@ -8273,13 +8260,13 @@
     <col customWidth="1" min="3" max="3" width="36.85546875"/>
     <col customWidth="1" min="4" max="4" style="8" width="38.85546875"/>
     <col customWidth="1" min="5" max="5" width="9.28515625"/>
-    <col customWidth="1" hidden="1" min="6" max="6" style="42" width="46.140625"/>
-    <col customWidth="1" min="7" max="7" style="42" width="19.5703125"/>
+    <col customWidth="1" hidden="1" min="6" max="6" style="41" width="46.140625"/>
+    <col customWidth="1" min="7" max="7" style="41" width="19.5703125"/>
     <col customWidth="1" min="8" max="8" width="12.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8287,7 +8274,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8295,42 +8282,42 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="72" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="72" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="72" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="73" t="s">
         <v>426</v>
       </c>
     </row>
@@ -8350,10 +8337,10 @@
       <c r="E9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="45" t="s">
         <v>58</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -8361,31 +8348,31 @@
       </c>
     </row>
     <row r="10" s="18" customFormat="1" ht="201.75" customHeight="1">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="54" t="s">
         <v>427</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>428</v>
       </c>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="55" t="s">
         <v>429</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="55" t="s">
         <v>430</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="57" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="56" t="s">
         <v>431</v>
       </c>
-      <c r="H10" s="75" t="s">
+      <c r="H10" s="74" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="11" s="23" customFormat="1" ht="71.25">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="58" t="s">
         <v>433</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -8394,14 +8381,14 @@
       <c r="C11" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="59" t="s">
         <v>435</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62" t="s">
+      <c r="F11" s="61"/>
+      <c r="G11" s="61" t="s">
         <v>436</v>
       </c>
       <c r="H11" s="18" t="s">
@@ -8409,7 +8396,7 @@
       </c>
     </row>
     <row r="12" s="23" customFormat="1" ht="142.5">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="58" t="s">
         <v>437</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -8418,14 +8405,14 @@
       <c r="C12" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="59" t="s">
         <v>439</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F12" s="62"/>
-      <c r="G12" s="62" t="s">
+      <c r="F12" s="61"/>
+      <c r="G12" s="61" t="s">
         <v>440</v>
       </c>
       <c r="H12" s="18" t="s">
@@ -8465,7 +8452,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8473,7 +8460,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -8481,15 +8468,15 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -8523,25 +8510,25 @@
       </c>
     </row>
     <row r="7" s="18" customFormat="1" ht="57">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="54" t="s">
         <v>445</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="56" t="s">
+      <c r="D7" s="55" t="s">
         <v>447</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="57" t="s">
+      <c r="F7" s="56" t="s">
         <v>448</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="56" t="s">
         <v>449</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -8549,25 +8536,25 @@
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="71.25">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="58" t="s">
         <v>450</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>451</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="75" t="s">
         <v>452</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="59" t="s">
         <v>453</v>
       </c>
       <c r="E8" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="59" t="s">
         <v>454</v>
       </c>
-      <c r="G8" s="61" t="s">
+      <c r="G8" s="60" t="s">
         <v>455</v>
       </c>
       <c r="H8" s="18" t="s">
@@ -8575,7 +8562,7 @@
       </c>
     </row>
     <row r="9" s="23" customFormat="1" ht="57">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="58" t="s">
         <v>456</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -8584,16 +8571,16 @@
       <c r="C9" s="23" t="s">
         <v>458</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="59" t="s">
         <v>459</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="59" t="s">
         <v>460</v>
       </c>
-      <c r="G9" s="61" t="s">
+      <c r="G9" s="60" t="s">
         <v>461</v>
       </c>
       <c r="H9" s="23" t="s">
@@ -8607,7 +8594,7 @@
       <c r="G10" s="9"/>
     </row>
     <row r="11" s="5" customFormat="1">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="69" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -8618,7 +8605,7 @@
       <c r="G11" s="9"/>
     </row>
     <row r="12" s="5" customFormat="1">
-      <c r="A12" s="70" t="s">
+      <c r="A12" s="69" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -8629,10 +8616,10 @@
       <c r="G12" s="9"/>
     </row>
     <row r="13" s="5" customFormat="1">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="76" t="s">
         <v>463</v>
       </c>
       <c r="D13" s="8"/>
@@ -8640,10 +8627,10 @@
       <c r="G13" s="9"/>
     </row>
     <row r="14" s="5" customFormat="1">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="76" t="s">
         <v>464</v>
       </c>
       <c r="D14" s="8"/>
@@ -8678,7 +8665,7 @@
       </c>
     </row>
     <row r="17" s="18" customFormat="1" ht="28.5">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="54" t="s">
         <v>465</v>
       </c>
       <c r="B17" s="18" t="s">
@@ -8687,14 +8674,14 @@
       <c r="C17" s="18" t="s">
         <v>467</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="55" t="s">
         <v>468</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57" t="s">
+      <c r="F17" s="56"/>
+      <c r="G17" s="56" t="s">
         <v>469</v>
       </c>
       <c r="H17" s="18" t="s">
@@ -8702,7 +8689,7 @@
       </c>
     </row>
     <row r="18" s="23" customFormat="1" ht="28.5">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="58" t="s">
         <v>470</v>
       </c>
       <c r="B18" s="23" t="s">
@@ -8711,14 +8698,14 @@
       <c r="C18" s="23" t="s">
         <v>467</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="59" t="s">
         <v>472</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61" t="s">
+      <c r="F18" s="60"/>
+      <c r="G18" s="60" t="s">
         <v>473</v>
       </c>
       <c r="H18" s="18" t="s">
@@ -8726,23 +8713,23 @@
       </c>
     </row>
     <row r="19" s="23" customFormat="1" ht="28.5">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="58" t="s">
         <v>474</v>
       </c>
       <c r="B19" s="23" t="s">
         <v>475</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>476</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61" t="s">
+      <c r="F19" s="60"/>
+      <c r="G19" s="60" t="s">
         <v>477</v>
       </c>
       <c r="H19" s="18" t="s">
@@ -8778,12 +8765,12 @@
     <col customWidth="1" min="3" max="3" width="26"/>
     <col customWidth="1" min="4" max="4" style="8" width="27.42578125"/>
     <col customWidth="1" min="5" max="5" width="9.7109375"/>
-    <col customWidth="1" hidden="1" min="6" max="6" style="42" width="46.140625"/>
-    <col customWidth="1" min="7" max="7" style="42" width="19.5703125"/>
+    <col customWidth="1" hidden="1" min="6" max="6" style="41" width="46.140625"/>
+    <col customWidth="1" min="7" max="7" style="41" width="19.5703125"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="42" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -8791,7 +8778,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -8799,10 +8786,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="73" t="s">
         <v>479</v>
       </c>
     </row>
@@ -8833,7 +8820,7 @@
       </c>
     </row>
     <row r="6" s="18" customFormat="1" ht="42.75">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="62" t="s">
         <v>263</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -8848,8 +8835,8 @@
       <c r="E6" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64" t="s">
+      <c r="F6" s="63"/>
+      <c r="G6" s="63" t="s">
         <v>481</v>
       </c>
       <c r="H6" s="18" t="s">
@@ -8857,7 +8844,7 @@
       </c>
     </row>
     <row r="7" s="23" customFormat="1" ht="42.75">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="70" t="s">
         <v>152</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -8872,8 +8859,8 @@
       <c r="E7" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="78"/>
-      <c r="G7" s="78" t="s">
+      <c r="F7" s="77"/>
+      <c r="G7" s="77" t="s">
         <v>483</v>
       </c>
       <c r="H7" s="18" t="s">
@@ -8881,7 +8868,7 @@
       </c>
     </row>
     <row r="8" s="23" customFormat="1" ht="42.75">
-      <c r="A8" s="71" t="s">
+      <c r="A8" s="70" t="s">
         <v>257</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -8896,8 +8883,8 @@
       <c r="E8" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78" t="s">
+      <c r="F8" s="77"/>
+      <c r="G8" s="77" t="s">
         <v>82</v>
       </c>
       <c r="H8" s="18" t="s">

</xml_diff>